<commit_message>
Changed optimal to corresponding in some cases
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7CB31E8A-8488-48B2-BBBC-ED875D52721B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4642F8C7-FE38-41E9-B442-B484951E86DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="48" windowWidth="23076" windowHeight="12192"/>
+    <workbookView xWindow="-36" yWindow="48" windowWidth="23076" windowHeight="12192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_Table" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Logistic Ridge Regression</t>
   </si>
   <si>
-    <t>optimal threshold</t>
-  </si>
-  <si>
     <t>optimal lambda</t>
   </si>
   <si>
@@ -64,42 +61,45 @@
     <t>optimal Area Under The Precision-Recall Curve</t>
   </si>
   <si>
-    <t>optimal accuracy</t>
-  </si>
-  <si>
-    <t>optimal True Positive Rate</t>
-  </si>
-  <si>
-    <t>optimate False Positive Rate</t>
-  </si>
-  <si>
-    <t>optimal precision</t>
+    <t>optimal Area Under The ROC Curve</t>
+  </si>
+  <si>
+    <t>value corresponding to optimal F1 measure</t>
+  </si>
+  <si>
+    <t>maximum average</t>
+  </si>
+  <si>
+    <t>K in sequence provided by Peter Gedeck corresponding to maximum F1 measure</t>
+  </si>
+  <si>
+    <t>lambda in sequence provided by glmnet::glmnet corresponding to maximum F1 measure</t>
+  </si>
+  <si>
+    <t>corresponding threshold</t>
+  </si>
+  <si>
+    <t>corresponding accuracy</t>
+  </si>
+  <si>
+    <t>corresponding True Positive Rate</t>
+  </si>
+  <si>
+    <t>corresponding False Positive Rate</t>
+  </si>
+  <si>
+    <t>corresponding precision</t>
   </si>
   <si>
     <t>optimal F1 measure</t>
-  </si>
-  <si>
-    <t>optimal Area Under The ROC Curve</t>
-  </si>
-  <si>
-    <t>value corresponding to optimal F1 measure</t>
-  </si>
-  <si>
-    <t>maximum average</t>
-  </si>
-  <si>
-    <t>K in sequence provided by Peter Gedeck corresponding to maximum F1 measure</t>
-  </si>
-  <si>
-    <t>lambda in sequence provided by glmnet::glmnet corresponding to maximum F1 measure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;???_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;???_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -611,13 +611,13 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -972,7 +972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1013,10 +1013,10 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2">
         <v>0.18</v>
@@ -1059,10 +1059,10 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -1082,10 +1082,10 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -1128,7 +1128,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -1151,10 +1151,10 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
       </c>
       <c r="D9" s="4">
         <v>0.996</v>
@@ -1174,10 +1174,10 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D10" s="4">
         <v>0.96599999999999997</v>
@@ -1197,10 +1197,10 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D11" s="6">
         <v>2.8400000000000001E-3</v>
@@ -1220,10 +1220,10 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D12" s="6">
         <v>0.91800000000000004</v>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D13" s="4">
         <v>0.94199999999999995</v>

</xml_diff>

<commit_message>
Set seed to ensure numbers are consistent. Talked about outputs naturally. Separated discussion of cross validation from bidirectional selection. Evaluated performance of Logistic Regression. Described warnings. Moved calculation of optimal lambda out of summarize_performance_of_cross_validated_models_using_dplyr. Described performance of optimal Logistic Ridge Regression, LDA, QDA, and KNN binary classifiers. Plotted the_cv.glmnet and list_of_[knn_]training_information. Revised comparison of models.
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4642F8C7-FE38-41E9-B442-B484951E86DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6199F2-9CF4-4914-93F2-DEB8326CDC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36" yWindow="48" windowWidth="23076" windowHeight="12192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_Table" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>K in sequence provided by Peter Gedeck corresponding to maximum F1 measure</t>
   </si>
   <si>
-    <t>lambda in sequence provided by glmnet::glmnet corresponding to maximum F1 measure</t>
-  </si>
-  <si>
     <t>corresponding threshold</t>
   </si>
   <si>
@@ -92,14 +89,18 @@
   </si>
   <si>
     <t>optimal F1 measure</t>
+  </si>
+  <si>
+    <t>lambda in sequence provided by glmnet::cv.glmnet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;???_);_(@_)"/>
+  <numFmts count="2">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;????_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -608,16 +609,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -981,11 +987,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="6.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="7.77734375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -995,42 +1001,42 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>0.18</v>
       </c>
-      <c r="E3" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.81100000000000005</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="E3" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="G3" s="3">
         <v>0.96</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="3">
         <v>0.08</v>
       </c>
     </row>
@@ -1041,19 +1047,19 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1062,21 +1068,21 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1087,20 +1093,20 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>3</v>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -1111,19 +1117,19 @@
         <v>5</v>
       </c>
       <c r="D7" s="4">
-        <v>0.98425200000000002</v>
+        <v>0.98440000000000005</v>
       </c>
       <c r="E7" s="5">
-        <v>0.96677579999999996</v>
+        <v>0.98109999999999997</v>
       </c>
       <c r="F7" s="6">
-        <v>0.9036843</v>
+        <v>0.90300000000000002</v>
       </c>
       <c r="G7" s="7">
-        <v>0.96531460000000002</v>
+        <v>0.96560000000000001</v>
       </c>
       <c r="H7" s="8">
-        <v>0.94301449999999998</v>
+        <v>0.94789999999999996</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
@@ -1134,134 +1140,134 @@
         <v>5</v>
       </c>
       <c r="D8" s="4">
-        <v>0.99921170000000004</v>
-      </c>
-      <c r="E8" s="7">
-        <v>0.99810759999999998</v>
+        <v>0.99929999999999997</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.99919999999999998</v>
       </c>
       <c r="F8" s="6">
-        <v>0.94973580000000002</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.99834009999999995</v>
+        <v>0.94940000000000002</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.99829999999999997</v>
       </c>
       <c r="H8" s="8">
-        <v>0.97348029999999997</v>
+        <v>0.97719999999999996</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4">
-        <v>0.996</v>
+      <c r="D9" s="5">
+        <v>0.99619999999999997</v>
       </c>
       <c r="E9" s="8">
-        <v>0.995</v>
+        <v>0.99570000000000003</v>
       </c>
       <c r="F9" s="6">
-        <v>0.99399999999999999</v>
+        <v>0.99370000000000003</v>
       </c>
       <c r="G9" s="7">
-        <v>0.996</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.996</v>
+        <v>0.99609999999999999</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.99650000000000005</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="4">
-        <v>0.96599999999999997</v>
+        <v>0.9667</v>
       </c>
       <c r="E10" s="8">
-        <v>0.90500000000000003</v>
+        <v>0.94440000000000002</v>
       </c>
       <c r="F10" s="6">
-        <v>0.81100000000000005</v>
+        <v>0.80969999999999998</v>
       </c>
       <c r="G10" s="7">
-        <v>0.93600000000000005</v>
+        <v>0.93689999999999996</v>
       </c>
       <c r="H10" s="5">
-        <v>0.93799999999999994</v>
+        <v>0.94569999999999999</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="6">
-        <v>2.8400000000000001E-3</v>
-      </c>
-      <c r="E11" s="7">
-        <v>1.99E-3</v>
-      </c>
-      <c r="F11" s="8">
-        <v>2.4499999999999999E-4</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1.9300000000000001E-3</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1.83E-3</v>
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1.9E-3</v>
+      </c>
+      <c r="H11" s="5">
+        <v>1.8E-3</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="6">
-        <v>0.91800000000000004</v>
+        <v>0.91790000000000005</v>
       </c>
       <c r="E12" s="8">
-        <v>0.93799999999999994</v>
+        <v>0.92320000000000002</v>
       </c>
       <c r="F12" s="4">
-        <v>0.99099999999999999</v>
+        <v>0.99160000000000004</v>
       </c>
       <c r="G12" s="7">
-        <v>0.94099999999999995</v>
+        <v>0.94120000000000004</v>
       </c>
       <c r="H12" s="5">
-        <v>0.94399999999999995</v>
+        <v>0.94610000000000005</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="4">
-        <v>0.94199999999999995</v>
+      <c r="D13" s="5">
+        <v>0.94120000000000004</v>
       </c>
       <c r="E13" s="8">
-        <v>0.92100000000000004</v>
+        <v>0.9335</v>
       </c>
       <c r="F13" s="6">
-        <v>0.89200000000000002</v>
+        <v>0.89119999999999999</v>
       </c>
       <c r="G13" s="7">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.94099999999999995</v>
+        <v>0.93889999999999996</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.94579999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expanded on nature and use of F1 measure. Calculated binary classifier scores. Recommended KNN binary classifier. Suggested using different F measures and choosing thresholds resulting in greater TPR. Recommended improvements.
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6199F2-9CF4-4914-93F2-DEB8326CDC38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3735D4CC-9435-4E25-A429-6F227B298223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23250" yWindow="75" windowWidth="23235" windowHeight="11115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_Table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>LDA</t>
   </si>
@@ -92,6 +92,24 @@
   </si>
   <si>
     <t>lambda in sequence provided by glmnet::cv.glmnet</t>
+  </si>
+  <si>
+    <t>weighted sum</t>
+  </si>
+  <si>
+    <t>binary-classifier score</t>
+  </si>
+  <si>
+    <t>lower bound of CI for optimal F1 measure</t>
+  </si>
+  <si>
+    <t>optimal F1 measure - critical t value * standard error of optimal F1 measure</t>
+  </si>
+  <si>
+    <t>upper bound of CI for optimal F1 measure</t>
+  </si>
+  <si>
+    <t>optimal F1 measure + critical t value * standard error of optimal F1 measure</t>
   </si>
 </sst>
 </file>
@@ -609,7 +627,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -624,6 +642,11 @@
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -979,19 +1002,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H13"/>
+  <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="42.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="7.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1270,6 +1293,80 @@
         <v>0.94579999999999997</v>
       </c>
     </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="5">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.8841</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.82940000000000003</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0.89139999999999997</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.90090000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.98809999999999998</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0.95299999999999996</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0.98650000000000004</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.99070000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="11">
+        <f>3*5+2*4+0*3+0*2+2*1</f>
+        <v>25</v>
+      </c>
+      <c r="E16" s="13">
+        <f>0*5+2*4+0*3+5*2+0*1</f>
+        <v>18</v>
+      </c>
+      <c r="F16" s="14">
+        <f>2*5+0*4+0*3+0*2+5*1</f>
+        <v>15</v>
+      </c>
+      <c r="G16" s="12">
+        <f>0*5+0*4+7*3+0*2+0*1</f>
+        <v>21</v>
+      </c>
+      <c r="H16" s="10">
+        <f>2*5+3*4+0*3+2*2+0*1</f>
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix: Redirected Precision-Recall curve to (1, min(Precision) = P/(N+P)). Added F1 measure, number of negatives, and number of positives to output of provide_performance_metrics. Added number of negatives and number of positives to data_frame_of_average_performance metrics and alphabetized attributes.
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3735D4CC-9435-4E25-A429-6F227B298223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB722DE-09E8-46A2-8EBE-272049CEF8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23250" yWindow="75" windowWidth="23235" windowHeight="11115" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24" yWindow="5688" windowWidth="23076" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_Table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>LDA</t>
   </si>
@@ -98,27 +98,16 @@
   </si>
   <si>
     <t>binary-classifier score</t>
-  </si>
-  <si>
-    <t>lower bound of CI for optimal F1 measure</t>
-  </si>
-  <si>
-    <t>optimal F1 measure - critical t value * standard error of optimal F1 measure</t>
-  </si>
-  <si>
-    <t>upper bound of CI for optimal F1 measure</t>
-  </si>
-  <si>
-    <t>optimal F1 measure + critical t value * standard error of optimal F1 measure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;????_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0000_);\(#,##0.0000\)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -627,7 +616,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -647,6 +636,7 @@
     <xf numFmtId="41" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="41" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="41" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1002,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H16"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,7 +1063,7 @@
       <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="15">
         <v>0</v>
       </c>
       <c r="F4" s="3">
@@ -1146,13 +1136,13 @@
         <v>0.98109999999999997</v>
       </c>
       <c r="F7" s="6">
-        <v>0.90300000000000002</v>
+        <v>0.90369999999999995</v>
       </c>
       <c r="G7" s="7">
         <v>0.96560000000000001</v>
       </c>
       <c r="H7" s="8">
-        <v>0.94789999999999996</v>
+        <v>0.9486</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
@@ -1278,7 +1268,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="5">
-        <v>0.94120000000000004</v>
+        <v>0.94159999999999999</v>
       </c>
       <c r="E13" s="8">
         <v>0.9335</v>
@@ -1295,74 +1285,28 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="E14" s="8">
-        <v>0.8841</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0.82940000000000003</v>
-      </c>
-      <c r="G14" s="7">
-        <v>0.89139999999999997</v>
-      </c>
-      <c r="H14" s="4">
-        <v>0.90090000000000003</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0.98809999999999998</v>
-      </c>
-      <c r="E15" s="8">
-        <v>0.98299999999999998</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0.95299999999999996</v>
-      </c>
-      <c r="G15" s="7">
-        <v>0.98650000000000004</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0.99070000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D14" s="11">
         <f>3*5+2*4+0*3+0*2+2*1</f>
         <v>25</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E14" s="13">
         <f>0*5+2*4+0*3+5*2+0*1</f>
         <v>18</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F14" s="14">
         <f>2*5+0*4+0*3+0*2+5*1</f>
         <v>15</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G14" s="12">
         <f>0*5+0*4+7*3+0*2+0*1</f>
         <v>21</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H14" s="10">
         <f>2*5+3*4+0*3+2*2+0*1</f>
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
Summarized performance of cross-validated KNN classifiers
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB722DE-09E8-46A2-8EBE-272049CEF8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A98A99-D2B8-4AE9-86F5-F04F47807A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24" yWindow="5688" windowWidth="23076" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1392" yWindow="960" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_Table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>LDA</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>binary-classifier score</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>SVMWLK</t>
   </si>
 </sst>
 </file>
@@ -245,7 +251,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,36 +429,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -616,7 +592,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -625,18 +601,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="41" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -992,22 +960,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:H14"/>
+  <dimension ref="B2:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1029,286 +998,287 @@
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    <row r="3" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="E3" s="5">
         <v>0.18</v>
       </c>
-      <c r="E3" s="3">
-        <v>0.18</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="F3" s="5">
         <v>0.69</v>
       </c>
-      <c r="G3" s="3">
-        <v>0.96</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.08</v>
+      <c r="G3" s="5">
+        <v>0.19</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+    <row r="4" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="15">
-        <v>0</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="5" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
         <v>1E-4</v>
       </c>
-      <c r="F5" s="3">
-        <v>0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+    <row r="6" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="9">
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+    <row r="7" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="4">
-        <v>0.98440000000000005</v>
+      <c r="D7" s="5">
+        <v>0.98380000000000001</v>
       </c>
       <c r="E7" s="5">
-        <v>0.98109999999999997</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0.90369999999999995</v>
-      </c>
-      <c r="G7" s="7">
-        <v>0.96560000000000001</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0.9486</v>
+        <v>0.98219999999999996</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.90449999999999997</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.95850000000000002</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.94850000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+    <row r="8" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4">
-        <v>0.99929999999999997</v>
+      <c r="D8" s="5">
+        <v>0.99919999999999998</v>
       </c>
       <c r="E8" s="5">
         <v>0.99919999999999998</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>0.94940000000000002</v>
       </c>
-      <c r="G8" s="7">
-        <v>0.99829999999999997</v>
-      </c>
-      <c r="H8" s="8">
+      <c r="G8" s="5">
+        <v>0.98470000000000002</v>
+      </c>
+      <c r="H8" s="5">
         <v>0.97719999999999996</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
+    <row r="9" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="5">
-        <v>0.99619999999999997</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0.99570000000000003</v>
-      </c>
-      <c r="F9" s="6">
+        <v>0.99590000000000001</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.996</v>
+      </c>
+      <c r="F9" s="5">
         <v>0.99370000000000003</v>
       </c>
-      <c r="G9" s="7">
-        <v>0.99609999999999999</v>
-      </c>
-      <c r="H9" s="4">
+      <c r="G9" s="5">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="H9" s="5">
         <v>0.99650000000000005</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="10" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="4">
-        <v>0.9667</v>
-      </c>
-      <c r="E10" s="8">
-        <v>0.94440000000000002</v>
-      </c>
-      <c r="F10" s="6">
-        <v>0.80969999999999998</v>
-      </c>
-      <c r="G10" s="7">
-        <v>0.93689999999999996</v>
+      <c r="D10" s="5">
+        <v>0.94110000000000005</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.81120000000000003</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.88770000000000004</v>
       </c>
       <c r="H10" s="5">
-        <v>0.94569999999999999</v>
+        <v>0.94550000000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+    <row r="11" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="6">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="E11" s="8">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="D11" s="5">
+        <v>2.3E-3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="F11" s="5">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="G11" s="7">
-        <v>1.9E-3</v>
+      <c r="G11" s="5">
+        <v>1.8E-3</v>
       </c>
       <c r="H11" s="5">
         <v>1.8E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+    <row r="12" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="6">
-        <v>0.91790000000000005</v>
-      </c>
-      <c r="E12" s="8">
-        <v>0.92320000000000002</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0.99160000000000004</v>
-      </c>
-      <c r="G12" s="7">
-        <v>0.94120000000000004</v>
+      <c r="D12" s="5">
+        <v>0.93010000000000004</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.92869999999999997</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.99109999999999998</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.94330000000000003</v>
       </c>
       <c r="H12" s="5">
-        <v>0.94610000000000005</v>
+        <v>0.94640000000000002</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+    <row r="13" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="5">
-        <v>0.94159999999999999</v>
-      </c>
-      <c r="E13" s="8">
-        <v>0.9335</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0.89119999999999999</v>
-      </c>
-      <c r="G13" s="7">
-        <v>0.93889999999999996</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0.94579999999999997</v>
+        <v>0.9355</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.89159999999999995</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.91449999999999998</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.94569999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="14" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="11">
-        <f>3*5+2*4+0*3+0*2+2*1</f>
-        <v>25</v>
-      </c>
-      <c r="E14" s="13">
-        <f>0*5+2*4+0*3+5*2+0*1</f>
-        <v>18</v>
-      </c>
-      <c r="F14" s="14">
-        <f>2*5+0*4+0*3+0*2+5*1</f>
-        <v>15</v>
-      </c>
-      <c r="G14" s="12">
-        <f>0*5+0*4+7*3+0*2+0*1</f>
-        <v>21</v>
-      </c>
-      <c r="H14" s="10">
-        <f>2*5+3*4+0*3+2*2+0*1</f>
-        <v>26</v>
+      <c r="D14" s="7">
+        <v>-1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>-1</v>
+      </c>
+      <c r="F14" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G14" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H14" s="7">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Summarized performance of cross-validated Support-Vector Machines with linear kernels
</commit_message>
<xml_diff>
--- a/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
+++ b/UVA/4--Statistical_Learning/Disaster_Relief_Project/Performance_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Tom_Levers_Public_Git_Repository\UVA\4--Statistical_Learning\Disaster_Relief_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A98A99-D2B8-4AE9-86F5-F04F47807A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77621A5-A8D7-4BCB-8936-A87FA9F748AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1392" yWindow="960" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="864" yWindow="408" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Performance_Table" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>LDA</t>
   </si>
@@ -70,9 +70,6 @@
     <t>maximum average</t>
   </si>
   <si>
-    <t>K in sequence provided by Peter Gedeck corresponding to maximum F1 measure</t>
-  </si>
-  <si>
     <t>corresponding threshold</t>
   </si>
   <si>
@@ -104,14 +101,38 @@
   </si>
   <si>
     <t>SVMWLK</t>
+  </si>
+  <si>
+    <t>optimal mtry</t>
+  </si>
+  <si>
+    <t>each number of predictors</t>
+  </si>
+  <si>
+    <t>optimal ntree</t>
+  </si>
+  <si>
+    <t>value less than 500 corresponding to optimal test error rate</t>
+  </si>
+  <si>
+    <t>optimal cost</t>
+  </si>
+  <si>
+    <t>K in sequence provided by Peter Gedeck
+corresponding to maximum F1 measure</t>
+  </si>
+  <si>
+    <t>cost in excerpt of sequence provided by Peter Gedeck
+corresponding to maximum F1 measure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;????_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000_);\(#,##0.0000\)"/>
   </numFmts>
@@ -601,10 +622,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -960,16 +983,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J14"/>
+  <dimension ref="B2:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.21875" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.44140625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="7.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -999,285 +1022,444 @@
         <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="1" t="s">
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.18</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.19</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="I3" s="7">
+        <v>0.46</v>
+      </c>
+      <c r="J3" s="7">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>2</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>47</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.98380000000000001</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.98219999999999996</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.90449999999999997</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.95850000000000002</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.94850000000000001</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.98629999999999995</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.98419999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.99919999999999998</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.99919999999999998</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.94940000000000002</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.98470000000000002</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.97719999999999996</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.99850000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.18</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0.69</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="D12" s="3">
+        <v>0.99590000000000001</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.996</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.99370000000000003</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.99470000000000003</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.99650000000000005</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.99719999999999998</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.99639999999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.94110000000000005</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.81120000000000003</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.88770000000000004</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.94550000000000001</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.9698</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.97030000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2.3E-3</v>
+      </c>
+      <c r="E14" s="3">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1.8E-3</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1.8E-3</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1.9E-3</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2.7000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.93010000000000004</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.92869999999999997</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.99109999999999998</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.94330000000000003</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.94640000000000002</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.94450000000000001</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.92149999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.9355</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.89159999999999995</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.91449999999999998</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.94569999999999999</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.95689999999999997</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.94520000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5">
-        <v>1E-4</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.98380000000000001</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0.98219999999999996</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.90449999999999997</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.95850000000000002</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.94850000000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.99919999999999998</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.99919999999999998</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.94940000000000002</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.98470000000000002</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.97719999999999996</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.99590000000000001</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.996</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.99370000000000003</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0.99470000000000003</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.99650000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.94110000000000005</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.94799999999999995</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0.81120000000000003</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0.88770000000000004</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0.94550000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="5">
-        <v>2.3E-3</v>
-      </c>
-      <c r="E11" s="5">
-        <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="F11" s="5">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1.8E-3</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1.8E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.93010000000000004</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.92869999999999997</v>
-      </c>
-      <c r="F12" s="5">
-        <v>0.99109999999999998</v>
-      </c>
-      <c r="G12" s="5">
-        <v>0.94330000000000003</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0.94640000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.9355</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.89159999999999995</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.91449999999999998</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.94569999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="7">
+      <c r="D17" s="5">
         <v>-1</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E17" s="5">
         <v>-1</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F17" s="5">
         <v>-1</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G17" s="5">
         <v>-1</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H17" s="5">
+        <v>-1</v>
+      </c>
+      <c r="I17" s="5">
+        <v>-1</v>
+      </c>
+      <c r="J17" s="5">
         <v>-1</v>
       </c>
     </row>

</xml_diff>